<commit_message>
outcomes_ath, 1_2_yearly_rep: att_age_ edR_age_, anR_age_, bnR_age_, bedR_age_ changed to decimal
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_2/1_2_yearly_rep.xlsx
+++ b/dictionaries/outcome_ath/1_2/1_2_yearly_rep.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\git_hub\dsUploadTest\20230831_uploadoutcomes11\dictMioMets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\git_hub\ds-dictionaries\dictionaries\outcome_ath\1_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274D23BE-C5E3-4376-A1A6-A74D4396B8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3389EF-B758-4A25-8004-ED3C176F55DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$87</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -94,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="207">
   <si>
     <t>name</t>
   </si>
@@ -754,7 +757,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,6 +767,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,12 +793,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="C61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B30:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,8 +1175,8 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1192,8 +1203,8 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1332,11 +1343,8 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
+      <c r="B16" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
@@ -1500,11 +1508,8 @@
       <c r="A28" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
+      <c r="B28" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D28" t="s">
         <v>60</v>
@@ -1542,11 +1547,8 @@
       <c r="A31" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
+      <c r="B31" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D31" t="s">
         <v>66</v>
@@ -1584,11 +1586,8 @@
       <c r="A34" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
+      <c r="B34" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D34" t="s">
         <v>72</v>
@@ -1626,11 +1625,8 @@
       <c r="A37" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
+      <c r="B37" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D37" t="s">
         <v>78</v>
@@ -2265,6 +2261,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D87" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="1">
     <dataValidation type="list" showErrorMessage="1" sqref="B5:B55" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"integer,decimal,text,binary,locale,boolean,datetime,date"</formula1>

</xml_diff>

<commit_message>
fix mets_score variables at 1_2 year_rep dict ath_outcome'
</commit_message>
<xml_diff>
--- a/dictionaries/outcome_ath/1_2/1_2_yearly_rep.xlsx
+++ b/dictionaries/outcome_ath/1_2/1_2_yearly_rep.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\git_hub\ds-dictionaries\dictionaries\outcome_ath\1_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3389EF-B758-4A25-8004-ED3C176F55DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06561A3-E4BD-46BE-8D1A-39EA3A27B401}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="209">
   <si>
     <t>name</t>
   </si>
@@ -718,6 +718,12 @@
   </si>
   <si>
     <t>Partial definition of MetS.  To have a definition of MetS also in those cohorts without information on fasting glucose or HOMA-IR.</t>
+  </si>
+  <si>
+    <t>mets_idefics_</t>
+  </si>
+  <si>
+    <t>mets_score_partial_idefics_</t>
   </si>
 </sst>
 </file>
@@ -1121,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B30:B31"/>
+    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,8 +1963,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>128</v>
+      <c r="A62" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
@@ -2250,8 +2256,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>205</v>
+      <c r="A87" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>

</xml_diff>